<commit_message>
Verified the utterance count between subsets
</commit_message>
<xml_diff>
--- a/data/Subset2_WithDialogActs/TalkBack.Year2.Strathom.Fall.102320.xlsx_with_dialog_acts.xlsx
+++ b/data/Subset2_WithDialogActs/TalkBack.Year2.Strathom.Fall.102320.xlsx_with_dialog_acts.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Teacher Tag</t>
   </si>
   <si>
-    <t xml:space="preserve">Speaker Tag</t>
+    <t xml:space="preserve">Student Tag</t>
   </si>
   <si>
     <t xml:space="preserve">DAMSLTag</t>
@@ -3072,10 +3072,13 @@
   <dimension ref="A1:J835"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.44"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">

</xml_diff>